<commit_message>
Add compressed CSV source data and ZIP support tools
- Added 4 compressed CSV archives (600MHz, 1000MHz, 1600MHz, 2000MHz)
- Total space savings: 238.5 MB  34.1 MB (85.7% compression)
- Added archive_csv_files.py for creating ZIP archives from network sources
- Added extract_data.py for extracting ZIP files when needed
- Added auto_analyzer_zip.py with dual support for network paths and ZIP files
- Added data/README.md with detailed usage instructions
- Updated analysis results with data source tracking
</commit_message>
<xml_diff>
--- a/output/master_summary.xlsx
+++ b/output/master_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,11 @@
           <t>Unique_Transitions</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Data_Source</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -534,6 +539,11 @@
       <c r="L2" t="n">
         <v>234844</v>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -574,6 +584,11 @@
       <c r="L3" t="n">
         <v>234844</v>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -614,6 +629,11 @@
       <c r="L4" t="n">
         <v>234844</v>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -653,6 +673,11 @@
       </c>
       <c r="L5" t="n">
         <v>234844</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>